<commit_message>
Tamsyn: doc edits, function edits
</commit_message>
<xml_diff>
--- a/Progress tracker.xlsx
+++ b/Progress tracker.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
   <si>
     <t>Function</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>This doesn't work with a list. Should we edit it so that it does?</t>
+  </si>
+  <si>
+    <t>homog_diag_boot</t>
   </si>
 </sst>
 </file>
@@ -698,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW361"/>
+  <dimension ref="A1:AW362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,29 +1087,43 @@
       <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="11"/>
+      <c r="B27" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="9"/>
+      <c r="B28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="9"/>
+        <v>55</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="9"/>
@@ -1114,7 +1131,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="9"/>
@@ -1122,7 +1139,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="9"/>
@@ -1130,7 +1147,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="9"/>
@@ -1138,7 +1155,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="9"/>
@@ -1146,7 +1163,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="9"/>
@@ -1154,7 +1171,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="9"/>
@@ -1162,7 +1179,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="9"/>
@@ -1170,7 +1187,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="9"/>
@@ -1178,14 +1195,16 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="9"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
+      <c r="A40" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="B40" s="6"/>
       <c r="C40" s="9"/>
       <c r="D40" s="11"/>
@@ -1912,6 +1931,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="4"/>
+      <c r="B161" s="6"/>
       <c r="C161" s="9"/>
       <c r="D161" s="11"/>
     </row>
@@ -2018,6 +2038,7 @@
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="4"/>
       <c r="C182" s="9"/>
+      <c r="D182" s="11"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="4"/>
@@ -2053,6 +2074,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="4"/>
+      <c r="C191" s="9"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="4"/>
@@ -2563,6 +2585,9 @@
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" s="4"/>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A362" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tamsyn: Added rest of Colin's functions, with documentation. Updated progress tracker
</commit_message>
<xml_diff>
--- a/Progress tracker.xlsx
+++ b/Progress tracker.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="68">
   <si>
     <t>Function</t>
   </si>
@@ -198,6 +198,42 @@
   </si>
   <si>
     <t>homog_diag_boot</t>
+  </si>
+  <si>
+    <t>Not needed</t>
+  </si>
+  <si>
+    <t>allfoil_ci_high</t>
+  </si>
+  <si>
+    <t>allfoil_ci_low</t>
+  </si>
+  <si>
+    <t>Ask about this code. Looks like it needs a table of bootstrapped data</t>
+  </si>
+  <si>
+    <t>gen_esize_m_ci</t>
+  </si>
+  <si>
+    <t>gen_esize_T_ci</t>
+  </si>
+  <si>
+    <t>How is this different to the function above?</t>
+  </si>
+  <si>
+    <t>gen_boot_propci</t>
+  </si>
+  <si>
+    <t>This function and the two below have exactly the same code</t>
+  </si>
+  <si>
+    <t>gen_boot_propmean_se</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>See comments in documentation re getting df of bootstrapped proportions</t>
   </si>
 </sst>
 </file>
@@ -367,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -387,6 +423,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,117 +1186,207 @@
       <c r="A32" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="9"/>
+      <c r="B34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="9"/>
+      <c r="B35" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D35" s="11"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D36" s="11"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="9"/>
+      <c r="B37" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="9"/>
+      <c r="B38" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D38" s="11"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="9"/>
+      <c r="B39" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="9"/>
+      <c r="B40" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D40" s="11"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="9"/>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D41" s="11"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="9"/>
+      <c r="E41" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D42" s="11"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="9"/>
+      <c r="E42" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D43" s="11"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="9"/>
+      <c r="E43" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="9"/>
+      <c r="E44" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D45" s="11"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="9"/>
+      <c r="E45" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="D46" s="11"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="6"/>
       <c r="C47" s="9"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="6"/>
       <c r="C48" s="9"/>

</xml_diff>

<commit_message>
Commit changes to Excel sheet
</commit_message>
<xml_diff>
--- a/Progress tracker.xlsx
+++ b/Progress tracker.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tamsyn Naylor\Documents\R Programming\lineupstat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\github\lineupstat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292EFD03-FE98-4F17-AA97-9D6E0C78E422}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions Progress" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="96">
   <si>
     <t>Function</t>
   </si>
@@ -144,103 +145,482 @@
     <t>No</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Have not looked at this function</t>
-  </si>
-  <si>
-    <t>Part of documentation (see: details) copied almost verbatim from Tredoux (1998, p. 234). Is this fine?</t>
-  </si>
-  <si>
-    <t>Make sure changes to this function reflect in other functions that call this one</t>
-  </si>
-  <si>
     <t>diag_param</t>
   </si>
   <si>
-    <t xml:space="preserve">Still needs some changes: 
-1.  We should probably add alpha option (choose some value other than 0.95, default in boot)
+    <t>General:</t>
+  </si>
+  <si>
+    <t>Change susp_pos to target_pos for all functions</t>
+  </si>
+  <si>
+    <t>In cases where we compute proportion for each lineup member, should I rather call the parameter 'member_pos' instead of 'target_pos'?</t>
+  </si>
+  <si>
+    <t>Package dependencies</t>
+  </si>
+  <si>
+    <t>tidyverse</t>
+  </si>
+  <si>
+    <t>magrittr</t>
+  </si>
+  <si>
+    <t>boot</t>
+  </si>
+  <si>
+    <t>homog_diag_boot</t>
+  </si>
+  <si>
+    <t>Not needed</t>
+  </si>
+  <si>
+    <t>allfoil_ci_high</t>
+  </si>
+  <si>
+    <t>allfoil_ci_low</t>
+  </si>
+  <si>
+    <t>gen_esize_m_ci</t>
+  </si>
+  <si>
+    <t>gen_esize_T_ci</t>
+  </si>
+  <si>
+    <t>gen_boot_propci</t>
+  </si>
+  <si>
+    <t>gen_boot_propmean_se</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>psych</t>
+  </si>
+  <si>
+    <t>ggrepel</t>
+  </si>
+  <si>
+    <t>pROC</t>
+  </si>
+  <si>
+    <t>GPArotation</t>
+  </si>
+  <si>
+    <t>magick</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>sim_face</t>
+  </si>
+  <si>
+    <t>show_lineup</t>
+  </si>
+  <si>
+    <t>Helper function</t>
+  </si>
+  <si>
+    <t>make_lineup_data</t>
+  </si>
+  <si>
+    <t>make_roc_data</t>
+  </si>
+  <si>
+    <t>make_roc_gg</t>
+  </si>
+  <si>
+    <t>make_roc</t>
+  </si>
+  <si>
+    <t>Reply</t>
+  </si>
+  <si>
+    <t>Yes. We might want to get someone to check</t>
+  </si>
+  <si>
+    <t>Need to - I think it is important</t>
+  </si>
+  <si>
+    <t>I don't think user needs to see this function?</t>
+  </si>
+  <si>
+    <t>Yes, add alpha as argument, offer Bonferonni etc</t>
+  </si>
+  <si>
+    <t>Have to check?</t>
+  </si>
+  <si>
+    <t>Does user call it?  Does it need to do lists?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Comments, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>plus replies</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Have not looked at this function.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I think we need this don't we?  Allows user to compute difference between two ES estimates</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Part of documentation (see: details) copied almost verbatim from Tredoux (1998, p. 234). Is this fine?  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FINE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Make sure changes to this function reflect in other functions that call this one; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Still needs some changes:  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I think these are my comments from earlier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1.  We should probably add alpha option (choose some value other than 0.95, default in boot)   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AGREED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 2.  We could offer alpha correction, too, since we are essentially doing k sig tests in that procedure.  What I mean is that we can add an argument allowing user to specify Bonferroni correction, or similar, and that would mean adjusting the CIs by simply adjusting the alpha argument.  Default would be FALSE
-3.  We could also make the bootstrap reps an argument
-4.  I am not sure about whether we should also bootstrap the overall function;probably should, and express the estimate as a 95% confidence interval.  
+3.  We could also make the bootstrap reps an argument  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+4.  I am not sure about whether we should also bootstrap the overall function;probably should, and express the estimate as a 95% confidence interval.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
-  </si>
-  <si>
-    <t>Part of documentation (see: details) copied almost verbatim from Tredoux (1998, p. 223). Is this fine?</t>
-  </si>
-  <si>
-    <t>General:</t>
-  </si>
-  <si>
-    <t>Change susp_pos to target_pos for all functions</t>
-  </si>
-  <si>
-    <t>In cases where we compute proportion for each lineup member, should I rather call the parameter 'member_pos' instead of 'target_pos'?</t>
-  </si>
-  <si>
-    <t>Package dependencies</t>
-  </si>
-  <si>
-    <t>tidyverse</t>
-  </si>
-  <si>
-    <t>magrittr</t>
-  </si>
-  <si>
-    <t>boot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One error msg: attempt to use zero-length variable name. Reran and error message disappeared, all worked fine. </t>
-  </si>
-  <si>
-    <t>This doesn't work with a list. Should we edit it so that it does?</t>
-  </si>
-  <si>
-    <t>homog_diag_boot</t>
-  </si>
-  <si>
-    <t>Not needed</t>
-  </si>
-  <si>
-    <t>allfoil_ci_high</t>
-  </si>
-  <si>
-    <t>allfoil_ci_low</t>
-  </si>
-  <si>
-    <t>Ask about this code. Looks like it needs a table of bootstrapped data</t>
-  </si>
-  <si>
-    <t>gen_esize_m_ci</t>
-  </si>
-  <si>
-    <t>gen_esize_T_ci</t>
-  </si>
-  <si>
-    <t>How is this different to the function above?</t>
-  </si>
-  <si>
-    <t>gen_boot_propci</t>
-  </si>
-  <si>
-    <t>This function and the two below have exactly the same code</t>
-  </si>
-  <si>
-    <t>gen_boot_propmean_se</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>See comments in documentation re getting df of bootstrapped proportions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Part of documentation (see: details) copied almost verbatim from Tredoux (1998, p. 223). Is this fine?  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OK</t>
+    </r>
+  </si>
+  <si>
+    <t>Part of documentation (see: details) copied almost verbatim from Tredoux (1998, p. 223). Is this fine?  OK</t>
+  </si>
+  <si>
+    <t>Part of documentation (see: details) copied almost verbatim from Tredoux (1998, p. 223). Is this fine? OK</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">One error msg: attempt to use zero-length variable name. Reran and error message disappeared, all worked fine.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sounds like it needs more checking</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This doesn't work with a list. Should we edit it so that it does?  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I think so</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Not nec to make it accessible </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>agreed</t>
+    </r>
+  </si>
+  <si>
+    <t>Not nec to make it accessible agreed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Might want to make it accessible, shows a lineup, useful </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YES, I THINK IT WOULD HELP USAGE TO SEE THE LINEUP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Experimental function; seems to work, needs checking on another computer etc.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YES&lt; NEED TO CHECK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ask about this code. Looks like it needs a table of bootstrapped data  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cant remember, but if so, yes.  But do we need to declare it, or reserve it</t>
+    </r>
+  </si>
+  <si>
+    <t>Ask about this code. Looks like it needs a table of bootstrapped data  cant remember, but if so, yes.  But do we need to declare it, or reserve it</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This function and the two below have exactly the same code </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>may be duplicate, keep them both but don't declare one</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">How is this different to the function above? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>See above comment</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">How is this different to the function above? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not sure that we need this anymore, but keep in the package and don't declare or document</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">See comments in documentation re getting df of bootstrapped proportions  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>can't look quite yet, will try later</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +646,30 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -737,11 +1141,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW362"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AW368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="F31" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,6 +1157,7 @@
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
     <col min="3" max="3" width="22.109375" customWidth="1"/>
     <col min="5" max="5" width="140" customWidth="1"/>
+    <col min="6" max="6" width="38.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="21" x14ac:dyDescent="0.4">
@@ -762,16 +1170,16 @@
     </row>
     <row r="3" spans="1:49" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:49" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.3">
@@ -794,9 +1202,11 @@
         <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -891,7 +1301,10 @@
       </c>
       <c r="D10" s="11"/>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.3">
@@ -918,12 +1331,15 @@
       </c>
       <c r="D12" s="11"/>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>37</v>
@@ -935,7 +1351,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.3">
@@ -974,10 +1390,13 @@
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
@@ -991,7 +1410,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1003,10 +1422,13 @@
       </c>
       <c r="D18" s="11"/>
       <c r="E18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
@@ -1018,10 +1440,13 @@
       </c>
       <c r="D19" s="11"/>
       <c r="E19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
@@ -1033,10 +1458,13 @@
       </c>
       <c r="D20" s="11"/>
       <c r="E20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -1048,7 +1476,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
@@ -1060,7 +1488,7 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1072,7 +1500,7 @@
       </c>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1086,10 +1514,13 @@
         <v>37</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -1103,7 +1534,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>22</v>
       </c>
@@ -1117,10 +1548,13 @@
         <v>37</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
@@ -1134,7 +1568,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
@@ -1146,9 +1580,9 @@
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>38</v>
@@ -1158,7 +1592,7 @@
       </c>
       <c r="D29" s="11"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>24</v>
       </c>
@@ -1170,7 +1604,7 @@
       </c>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
@@ -1182,7 +1616,7 @@
       </c>
       <c r="D31" s="11"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>27</v>
       </c>
@@ -1232,43 +1666,52 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D36" s="11"/>
+      <c r="E36" s="16" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D37" s="11"/>
+      <c r="E37" s="16" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D38" s="11"/>
+      <c r="E38" s="16" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>37</v>
@@ -1277,10 +1720,11 @@
         <v>37</v>
       </c>
       <c r="D39" s="11"/>
+      <c r="E39" s="16"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>37</v>
@@ -1292,37 +1736,34 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D41" s="11"/>
-      <c r="E41" s="16" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="16" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>37</v>
@@ -1332,157 +1773,202 @@
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="16" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D44" s="11"/>
-      <c r="E44" s="16" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D45" s="11"/>
-      <c r="E45" s="16" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>66</v>
+        <v>35</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="D46" s="11"/>
-      <c r="E46" s="16" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="9"/>
+      <c r="A47" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D47" s="11"/>
+      <c r="E47" s="16" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="9"/>
+      <c r="A48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D48" s="11"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="4"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="9"/>
+      <c r="E48" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="9"/>
+      <c r="E49" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="4"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="9"/>
+      <c r="E50" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D51" s="11"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="4"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="9"/>
+      <c r="E51" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="D52" s="11"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="6"/>
       <c r="C53" s="9"/>
       <c r="D53" s="11"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="6"/>
       <c r="C54" s="9"/>
       <c r="D54" s="11"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="6"/>
       <c r="C55" s="9"/>
       <c r="D55" s="11"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="6"/>
       <c r="C56" s="9"/>
       <c r="D56" s="11"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="6"/>
       <c r="C57" s="9"/>
       <c r="D57" s="11"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="6"/>
       <c r="C58" s="9"/>
       <c r="D58" s="11"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="6"/>
       <c r="C59" s="9"/>
       <c r="D59" s="11"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="6"/>
       <c r="C60" s="9"/>
       <c r="D60" s="11"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="6"/>
       <c r="C61" s="9"/>
       <c r="D61" s="11"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="6"/>
       <c r="C62" s="9"/>
       <c r="D62" s="11"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="6"/>
       <c r="C63" s="9"/>
       <c r="D63" s="11"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="6"/>
       <c r="C64" s="9"/>
@@ -2072,31 +2558,37 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="4"/>
+      <c r="B162" s="6"/>
       <c r="C162" s="9"/>
       <c r="D162" s="11"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="4"/>
+      <c r="B163" s="6"/>
       <c r="C163" s="9"/>
       <c r="D163" s="11"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="4"/>
+      <c r="B164" s="6"/>
       <c r="C164" s="9"/>
       <c r="D164" s="11"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="4"/>
+      <c r="B165" s="6"/>
       <c r="C165" s="9"/>
       <c r="D165" s="11"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="4"/>
+      <c r="B166" s="6"/>
       <c r="C166" s="9"/>
       <c r="D166" s="11"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="4"/>
+      <c r="B167" s="6"/>
       <c r="C167" s="9"/>
       <c r="D167" s="11"/>
     </row>
@@ -2178,26 +2670,32 @@
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="4"/>
       <c r="C183" s="9"/>
+      <c r="D183" s="11"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="4"/>
       <c r="C184" s="9"/>
+      <c r="D184" s="11"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="4"/>
       <c r="C185" s="9"/>
+      <c r="D185" s="11"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="4"/>
       <c r="C186" s="9"/>
+      <c r="D186" s="11"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="4"/>
       <c r="C187" s="9"/>
+      <c r="D187" s="11"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="4"/>
       <c r="C188" s="9"/>
+      <c r="D188" s="11"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="4"/>
@@ -2213,53 +2711,59 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="4"/>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C192" s="9"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="4"/>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C193" s="9"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="4"/>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C194" s="9"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="4"/>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C195" s="9"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="4"/>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C196" s="9"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="4"/>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C197" s="9"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="4"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="4"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="4"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="4"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="4"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="4"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="4"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="4"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="4"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="4"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="4"/>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
@@ -2723,6 +3227,24 @@
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" s="4"/>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A363" s="4"/>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A364" s="4"/>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A365" s="4"/>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A366" s="4"/>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A367" s="4"/>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A368" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2731,11 +3253,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2745,22 +3267,52 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>